<commit_message>
Fix errors in rev1
</commit_message>
<xml_diff>
--- a/pcb/BOM.xlsx
+++ b/pcb/BOM.xlsx
@@ -103,7 +103,7 @@
     <t xml:space="preserve">Spacers, 11mm</t>
   </si>
   <si>
-    <t xml:space="preserve">R1</t>
+    <t xml:space="preserve">R1-R2</t>
   </si>
   <si>
     <t xml:space="preserve">ERJ-8ENF1002V</t>
@@ -355,7 +355,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>